<commit_message>
Revert "Virtual Devices Added"
This reverts commit f8aaf7d64cb949a61ac794ed5e62df26ddfce723.
</commit_message>
<xml_diff>
--- a/src/Data.xlsx
+++ b/src/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bridgette\React\fog-server\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8C27D9-7B9B-4CFE-8511-975ED857FC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE587A5-E195-4B98-AEFD-61FB3BDFB2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="159">
   <si>
     <t>Id</t>
   </si>
@@ -517,15 +517,6 @@
   </si>
   <si>
     <t>Unregistered Device</t>
-  </si>
-  <si>
-    <t>Virtual-Device-1</t>
-  </si>
-  <si>
-    <t>Virtual-Device-2</t>
-  </si>
-  <si>
-    <t>Virtual-Device-3</t>
   </si>
 </sst>
 </file>
@@ -553,18 +544,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -579,12 +564,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1170,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1212,7 +1196,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1238,7 +1222,7 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -1801,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A598F70-FCF0-43CC-B496-2B7952A42844}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,7 +2155,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -2209,7 +2193,7 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -2247,7 +2231,7 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -2973,8 +2957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3C0614-E23F-4957-ABD5-C6B390DAE333}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+    <sheetView topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3487,8 +3471,8 @@
       <c r="D11" t="s">
         <v>147</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>159</v>
+      <c r="E11" t="s">
+        <v>51</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
@@ -3535,7 +3519,7 @@
         <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
@@ -3581,8 +3565,8 @@
       <c r="D13" t="s">
         <v>147</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>161</v>
+      <c r="E13" t="s">
+        <v>53</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -4526,8 +4510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF08B535-1CD7-4839-8A41-B9B36E203083}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4811,7 +4795,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>51</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -4840,7 +4824,7 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -4869,7 +4853,7 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>53</v>
       </c>
       <c r="E12">
         <v>10</v>

</xml_diff>

<commit_message>
Update to Devices in Dashboard
</commit_message>
<xml_diff>
--- a/src/Data.xlsx
+++ b/src/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bridgette\React\fog-server\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB9AEF2-EED0-448A-9AA8-8DF8B582A439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619A2172-8F5B-495A-98C4-5B4A259F7311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="595" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Devices" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="174">
   <si>
     <t>Id</t>
   </si>
@@ -550,6 +550,18 @@
   </si>
   <si>
     <t>Ok</t>
+  </si>
+  <si>
+    <t>DTYPE</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Unregistered</t>
   </si>
 </sst>
 </file>
@@ -627,9 +639,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8DC48D6-6481-45B4-9ACB-B76CA38BC59E}" name="Table1" displayName="Table1" ref="A1:K33" totalsRowShown="0">
-  <autoFilter ref="A1:K33" xr:uid="{B8DC48D6-6481-45B4-9ACB-B76CA38BC59E}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8DC48D6-6481-45B4-9ACB-B76CA38BC59E}" name="Table1" displayName="Table1" ref="A1:L33" totalsRowShown="0">
+  <autoFilter ref="A1:L33" xr:uid="{B8DC48D6-6481-45B4-9ACB-B76CA38BC59E}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{8139FF78-45D2-45B9-AF65-44FCBEB4704F}" name="Id"/>
     <tableColumn id="2" xr3:uid="{CCF64B95-81ED-47B2-9D67-CDE5AD2E6261}" name="IP"/>
     <tableColumn id="3" xr3:uid="{9C909E5A-BC40-4C7A-B78C-767450E56D61}" name="Name"/>
@@ -641,6 +653,7 @@
     <tableColumn id="6" xr3:uid="{FFF548D7-4102-4697-9A9A-542DC93CC1AF}" name="Status"/>
     <tableColumn id="7" xr3:uid="{8B3EC318-A669-4ACD-A2E2-0C0AB73BDC29}" name="State"/>
     <tableColumn id="8" xr3:uid="{D536F729-79FF-456E-B521-D08D5009198C}" name="Registered"/>
+    <tableColumn id="12" xr3:uid="{459B051A-BC94-4CF5-A7AC-8786DCB9F858}" name="DTYPE"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -947,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,9 +975,10 @@
     <col min="5" max="8" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -998,8 +1012,11 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -1033,8 +1050,11 @@
       <c r="K2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -1068,8 +1088,11 @@
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1103,8 +1126,11 @@
       <c r="K4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -1138,8 +1164,11 @@
       <c r="K5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1173,8 +1202,11 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1208,8 +1240,11 @@
       <c r="K7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1243,8 +1278,11 @@
       <c r="K8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -1278,8 +1316,11 @@
       <c r="K9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -1313,8 +1354,11 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -1348,8 +1392,11 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -1383,8 +1430,11 @@
       <c r="K12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -1418,8 +1468,11 @@
       <c r="K13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>97</v>
       </c>
@@ -1453,8 +1506,11 @@
       <c r="K14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -1488,8 +1544,11 @@
       <c r="K15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -1523,8 +1582,11 @@
       <c r="K16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -1558,8 +1620,11 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -1593,8 +1658,11 @@
       <c r="K18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>102</v>
       </c>
@@ -1628,8 +1696,11 @@
       <c r="K19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>103</v>
       </c>
@@ -1663,8 +1734,11 @@
       <c r="K20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -1698,8 +1772,11 @@
       <c r="K21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>105</v>
       </c>
@@ -1733,8 +1810,11 @@
       <c r="K22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -1768,8 +1848,11 @@
       <c r="K23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -1803,8 +1886,11 @@
       <c r="K24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -1838,8 +1924,11 @@
       <c r="K25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -1873,8 +1962,11 @@
       <c r="K26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -1908,8 +2000,11 @@
       <c r="K27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -1943,8 +2038,11 @@
       <c r="K28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -1978,8 +2076,11 @@
       <c r="K29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -2013,8 +2114,11 @@
       <c r="K30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2039,8 +2143,11 @@
       <c r="K31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -2065,8 +2172,11 @@
       <c r="K32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2090,6 +2200,9 @@
       </c>
       <c r="K33" t="b">
         <v>0</v>
+      </c>
+      <c r="L33" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2170,7 +2283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A598F70-FCF0-43CC-B496-2B7952A42844}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>